<commit_message>
Updated project plan and initial html
</commit_message>
<xml_diff>
--- a/Documentation/Project 3 Plan.xlsx
+++ b/Documentation/Project 3 Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{2DA2D03C-5B49-49AE-8935-CBC014F4D906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A008FB-A8F1-4C70-9ECB-D7C74B5B00FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -532,7 +532,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -575,13 +575,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -600,6 +600,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="11" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="4" applyBorder="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="9" applyBorder="1">
@@ -607,27 +625,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="11" applyBorder="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="4" applyBorder="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -920,7 +917,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -934,12 +931,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="2:17" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -960,72 +957,72 @@
       <c r="M2" s="12"/>
     </row>
     <row r="3" spans="2:17" s="4" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
     </row>
     <row r="4" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="29">
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="26">
         <v>45390</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="26">
         <v>45391</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="26">
         <v>45392</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="26">
         <v>45393</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="26">
         <v>45394</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="26">
         <v>45395</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4" s="26">
         <v>45396</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="26">
         <v>45397</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="26">
         <v>45398</v>
       </c>
-      <c r="P4" s="29">
+      <c r="P4" s="26">
         <v>45399</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="Q4" s="26">
         <v>45400</v>
       </c>
     </row>
@@ -1075,7 +1072,7 @@
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="20"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="18"/>
       <c r="K6" s="19"/>
       <c r="L6" s="18"/>
@@ -1096,14 +1093,14 @@
         <v>45392</v>
       </c>
       <c r="E7" s="15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="17"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="18"/>
       <c r="K7" s="19"/>
       <c r="L7" s="18"/>
@@ -1152,14 +1149,14 @@
         <v>45392</v>
       </c>
       <c r="E9" s="15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="17"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="18"/>
       <c r="K9" s="19"/>
       <c r="L9" s="18"/>
@@ -1180,14 +1177,14 @@
         <v>45392</v>
       </c>
       <c r="E10" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="18"/>
       <c r="K10" s="19"/>
       <c r="L10" s="18"/>

</xml_diff>

<commit_message>
Corrected fileClean.py and initial plotting
</commit_message>
<xml_diff>
--- a/Documentation/Project 3 Plan.xlsx
+++ b/Documentation/Project 3 Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A008FB-A8F1-4C70-9ECB-D7C74B5B00FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC95B45-601F-4188-B521-BC0EEA6F34D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>PERIODS</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Visualization Design</t>
-  </si>
-  <si>
-    <t>Flask Server (API)</t>
   </si>
   <si>
     <t>Visualization Page</t>
@@ -917,7 +914,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1121,14 +1118,14 @@
         <v>45392</v>
       </c>
       <c r="E8" s="15">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="17"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="18"/>
       <c r="K8" s="19"/>
       <c r="L8" s="18"/>
@@ -1205,16 +1202,16 @@
         <v>45394</v>
       </c>
       <c r="E11" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="18"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
       <c r="L11" s="18"/>
       <c r="M11" s="19"/>
       <c r="N11" s="18"/>
@@ -1224,51 +1221,51 @@
     </row>
     <row r="12" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="14">
-        <v>45392</v>
+        <v>45393</v>
       </c>
       <c r="D12" s="14">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="E12" s="15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="18"/>
-      <c r="I12" s="20"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="18"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
       <c r="Q12" s="19"/>
     </row>
     <row r="13" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" s="14">
-        <v>45393</v>
+        <v>45396</v>
       </c>
       <c r="D13" s="14">
-        <v>45399</v>
+        <v>45398</v>
       </c>
       <c r="E13" s="15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="18"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -1283,38 +1280,38 @@
         <v>21</v>
       </c>
       <c r="C14" s="14">
-        <v>45396</v>
+        <v>45394</v>
       </c>
       <c r="D14" s="14">
-        <v>45398</v>
+        <v>45397</v>
       </c>
       <c r="E14" s="15">
         <v>0</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="18"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="18"/>
       <c r="Q14" s="19"/>
     </row>
     <row r="15" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="14">
-        <v>45394</v>
+        <v>45398</v>
       </c>
       <c r="D15" s="14">
-        <v>45397</v>
+        <v>45399</v>
       </c>
       <c r="E15" s="15">
         <v>0</v>
@@ -1326,12 +1323,12 @@
       <c r="H15" s="18"/>
       <c r="I15" s="19"/>
       <c r="J15" s="18"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="18"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="19"/>
     </row>
     <row r="16" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1339,25 +1336,25 @@
         <v>24</v>
       </c>
       <c r="C16" s="14">
-        <v>45398</v>
+        <v>45399</v>
       </c>
       <c r="D16" s="14">
         <v>45399</v>
       </c>
       <c r="E16" s="15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="18"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="19"/>
@@ -1376,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="18"/>
@@ -1395,10 +1392,10 @@
         <v>26</v>
       </c>
       <c r="C18" s="14">
-        <v>45399</v>
+        <v>45400</v>
       </c>
       <c r="D18" s="14">
-        <v>45399</v>
+        <v>45400</v>
       </c>
       <c r="E18" s="15">
         <v>0</v>
@@ -1415,37 +1412,10 @@
       <c r="M18" s="19"/>
       <c r="N18" s="18"/>
       <c r="O18" s="19"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="19"/>
-    </row>
-    <row r="19" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="14">
-        <v>45400</v>
-      </c>
-      <c r="D19" s="14">
-        <v>45400</v>
-      </c>
-      <c r="E19" s="15">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="20"/>
-    </row>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="20"/>
+    </row>
+    <row r="19" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B3:B4"/>

</xml_diff>

<commit_message>
Stock data json and new viz layout
</commit_message>
<xml_diff>
--- a/Documentation/Project 3 Plan.xlsx
+++ b/Documentation/Project 3 Plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC95B45-601F-4188-B521-BC0EEA6F34D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5485EE09-D254-4308-AE7B-A3FBD5F55253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="468" windowWidth="21264" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -913,8 +913,8 @@
   <dimension ref="B1:Q19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1238,7 +1238,7 @@
       <c r="G12" s="19"/>
       <c r="H12" s="18"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="20"/>
+      <c r="J12" s="17"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
@@ -1266,7 +1266,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="18"/>
       <c r="I13" s="17"/>
-      <c r="J13" s="20"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
@@ -1294,7 +1294,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
@@ -1350,7 +1350,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="20"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>

</xml_diff>

<commit_message>
Added Apex charts, readme and plan updates.
</commit_message>
<xml_diff>
--- a/Documentation/Project 3 Plan.xlsx
+++ b/Documentation/Project 3 Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5485EE09-D254-4308-AE7B-A3FBD5F55253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7295F64E-4BB6-4120-8EEC-BDEC7F383851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="348" yWindow="468" windowWidth="21264" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -914,7 +914,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1239,9 +1239,9 @@
       <c r="H12" s="18"/>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
@@ -1267,9 +1267,9 @@
       <c r="H13" s="18"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
@@ -1295,9 +1295,9 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
       <c r="J14" s="17"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
       <c r="N14" s="20"/>
       <c r="O14" s="19"/>
       <c r="P14" s="18"/>
@@ -1351,10 +1351,10 @@
       <c r="H16" s="18"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="19"/>

</xml_diff>

<commit_message>
Format updates for cash flow currency
</commit_message>
<xml_diff>
--- a/Documentation/Project 3 Plan.xlsx
+++ b/Documentation/Project 3 Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7295F64E-4BB6-4120-8EEC-BDEC7F383851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F67403-53CA-4B73-AF14-06E21A3BCD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="348" yWindow="468" windowWidth="21264" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -914,7 +914,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1230,7 +1230,7 @@
         <v>45399</v>
       </c>
       <c r="E12" s="15">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>17</v>
@@ -1242,8 +1242,8 @@
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="19"/>
     </row>
@@ -1258,7 +1258,7 @@
         <v>45398</v>
       </c>
       <c r="E13" s="15">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>13</v>
@@ -1270,8 +1270,8 @@
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="19"/>
     </row>
@@ -1286,7 +1286,7 @@
         <v>45397</v>
       </c>
       <c r="E14" s="15">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>15</v>
@@ -1298,7 +1298,7 @@
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
-      <c r="N14" s="20"/>
+      <c r="N14" s="17"/>
       <c r="O14" s="19"/>
       <c r="P14" s="18"/>
       <c r="Q14" s="19"/>
@@ -1342,7 +1342,7 @@
         <v>45399</v>
       </c>
       <c r="E16" s="15">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Layout change for logo, horizontal
</commit_message>
<xml_diff>
--- a/Documentation/Project 3 Plan.xlsx
+++ b/Documentation/Project 3 Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F67403-53CA-4B73-AF14-06E21A3BCD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D129C83A-AB7A-4BBD-A310-CA877599FB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="348" yWindow="468" windowWidth="21264" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,7 +276,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,12 +337,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor auto="1"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="gray0625">
         <fgColor auto="1"/>
         <bgColor theme="4" tint="0.39994506668294322"/>
@@ -529,7 +523,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -581,7 +575,7 @@
     <xf numFmtId="9" fontId="14" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -590,13 +584,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="11" applyBorder="1">
@@ -914,7 +905,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -928,12 +919,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="2:17" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -941,12 +932,12 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="21"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="8"/>
-      <c r="J2" s="22"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="10" t="s">
         <v>2</v>
       </c>
@@ -954,72 +945,72 @@
       <c r="M2" s="12"/>
     </row>
     <row r="3" spans="2:17" s="4" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
     </row>
     <row r="4" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="26">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="25">
         <v>45390</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="25">
         <v>45391</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="25">
         <v>45392</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <v>45393</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="25">
         <v>45394</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="25">
         <v>45395</v>
       </c>
-      <c r="M4" s="26">
+      <c r="M4" s="25">
         <v>45396</v>
       </c>
-      <c r="N4" s="26">
+      <c r="N4" s="25">
         <v>45397</v>
       </c>
-      <c r="O4" s="26">
+      <c r="O4" s="25">
         <v>45398</v>
       </c>
-      <c r="P4" s="26">
+      <c r="P4" s="25">
         <v>45399</v>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="25">
         <v>45400</v>
       </c>
     </row>
@@ -1230,7 +1221,7 @@
         <v>45399</v>
       </c>
       <c r="E12" s="15">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>17</v>
@@ -1244,7 +1235,7 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
-      <c r="P12" s="20"/>
+      <c r="P12" s="17"/>
       <c r="Q12" s="19"/>
     </row>
     <row r="13" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1258,7 +1249,7 @@
         <v>45398</v>
       </c>
       <c r="E13" s="15">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>13</v>
@@ -1272,7 +1263,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
-      <c r="P13" s="20"/>
+      <c r="P13" s="17"/>
       <c r="Q13" s="19"/>
     </row>
     <row r="14" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1286,7 +1277,7 @@
         <v>45397</v>
       </c>
       <c r="E14" s="15">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>15</v>
@@ -1314,7 +1305,7 @@
         <v>45399</v>
       </c>
       <c r="E15" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>15</v>
@@ -1327,8 +1318,8 @@
       <c r="L15" s="18"/>
       <c r="M15" s="19"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
       <c r="Q15" s="19"/>
     </row>
     <row r="16" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1342,7 +1333,7 @@
         <v>45399</v>
       </c>
       <c r="E16" s="15">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>13</v>
@@ -1355,8 +1346,8 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
       <c r="Q16" s="19"/>
     </row>
     <row r="17" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1370,7 +1361,7 @@
         <v>45399</v>
       </c>
       <c r="E17" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>12</v>
@@ -1384,7 +1375,7 @@
       <c r="M17" s="19"/>
       <c r="N17" s="18"/>
       <c r="O17" s="19"/>
-      <c r="P17" s="20"/>
+      <c r="P17" s="17"/>
       <c r="Q17" s="19"/>
     </row>
     <row r="18" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1398,7 +1389,7 @@
         <v>45400</v>
       </c>
       <c r="E18" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>12</v>
@@ -1413,7 +1404,7 @@
       <c r="N18" s="18"/>
       <c r="O18" s="19"/>
       <c r="P18" s="18"/>
-      <c r="Q18" s="20"/>
+      <c r="Q18" s="17"/>
     </row>
     <row r="19" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>